<commit_message>
actualizando bloques a fecha actual
</commit_message>
<xml_diff>
--- a/blocks/inventarios/gestionActa/registrarElementoActa/plantilla/archivo_elementos.xlsx
+++ b/blocks/inventarios/gestionActa/registrarElementoActa/plantilla/archivo_elementos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="504" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Datos a Cargar" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,11 @@
     <sheet name="Marca y Serie " sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -879,20 +884,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.015306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.8316326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,20 +974,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.015306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1020408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9387755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.8316326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,20 +1186,20 @@
   </sheetPr>
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.0969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.1632653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,17 +2838,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,6 +2905,14 @@
       </c>
       <c r="B7" s="21" t="n">
         <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="21" t="n">
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>
@@ -2926,13 +2939,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="23.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="11.3418367346939"/>
     <col collapsed="false" hidden="true" max="9" min="9" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="36.9540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,10 +3035,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3979591836735"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>